<commit_message>
Worked on Filter Panel
</commit_message>
<xml_diff>
--- a/my-app/src/components/Products/productdata.xlsx
+++ b/my-app/src/components/Products/productdata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Samuel Ho\Dropbox\Coding Projects\Streetwear Website - React\my-app\src\components\Products\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{086B6EDB-7E18-40D8-8D0D-B7781EE31C30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF1A54CC-5736-4CFB-8E40-D8032B26B7CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{6C4069A5-B8E7-4026-BF0A-47BF496EED05}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="productdata" sheetId="2" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="ExternalData_1" localSheetId="0" hidden="1">productdata!$A$1:$G$20</definedName>
+    <definedName name="ExternalData_1" localSheetId="0" hidden="1">productdata!$B$1:$H$20</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="77">
   <si>
     <t>product-name</t>
   </si>
@@ -274,6 +274,9 @@
   </si>
   <si>
     <t>Abby Hoodie</t>
+  </si>
+  <si>
+    <t>id</t>
   </si>
 </sst>
 </file>
@@ -330,8 +333,9 @@
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="ExternalData_1" connectionId="1" xr16:uid="{458F97E8-F58D-4AE9-B708-422214DC2E84}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0">
-  <queryTableRefresh nextId="9">
-    <queryTableFields count="7">
+  <queryTableRefresh nextId="10" unboundColumnsLeft="1">
+    <queryTableFields count="8">
+      <queryTableField id="9" dataBound="0" tableColumnId="8"/>
       <queryTableField id="1" name="product-name" tableColumnId="1"/>
       <queryTableField id="2" name="designer" tableColumnId="2"/>
       <queryTableField id="7" dataBound="0" tableColumnId="7"/>
@@ -345,9 +349,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{7BB60203-6409-4C86-BAD9-5B9526BA1841}" name="productdata" displayName="productdata" ref="A1:G20" tableType="queryTable" totalsRowShown="0">
-  <autoFilter ref="A1:G20" xr:uid="{7BB60203-6409-4C86-BAD9-5B9526BA1841}"/>
-  <tableColumns count="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{7BB60203-6409-4C86-BAD9-5B9526BA1841}" name="productdata" displayName="productdata" ref="A1:H20" tableType="queryTable" totalsRowShown="0">
+  <autoFilter ref="A1:H20" xr:uid="{7BB60203-6409-4C86-BAD9-5B9526BA1841}"/>
+  <tableColumns count="8">
+    <tableColumn id="8" xr3:uid="{03004C07-7EA5-443D-9E66-AF30C79A71D7}" uniqueName="8" name="id" queryTableFieldId="9"/>
     <tableColumn id="1" xr3:uid="{B3E2DD71-C516-427D-953D-E9CFC32BF28B}" uniqueName="1" name="product-name" queryTableFieldId="1"/>
     <tableColumn id="2" xr3:uid="{D4A6FF33-8AA6-4310-B7E1-DF1074BAB156}" uniqueName="2" name="designer" queryTableFieldId="2"/>
     <tableColumn id="7" xr3:uid="{2D2986F1-D384-4164-9D5B-002932F5E704}" uniqueName="7" name="category" queryTableFieldId="7"/>
@@ -657,15 +662,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E7A261A-3C28-4627-8248-D088B4D65DCE}">
-  <dimension ref="A1:G20"/>
+  <dimension ref="A1:H20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="4.77734375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="31.5546875" customWidth="1"/>
     <col min="3" max="3" width="7.44140625" customWidth="1"/>
     <col min="4" max="4" width="7" bestFit="1" customWidth="1"/>
@@ -675,463 +680,523 @@
     <col min="8" max="8" width="7.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>11</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
         <v>7</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>15</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>12</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>55</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>61</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>6</v>
       </c>
-      <c r="G2">
+      <c r="H2">
         <v>240</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
         <v>8</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>15</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>12</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>55</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>61</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>6</v>
       </c>
-      <c r="G3">
+      <c r="H3">
         <v>200</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
         <v>75</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>15</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>12</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>55</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
         <v>61</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G4" t="s">
         <v>6</v>
       </c>
-      <c r="G4">
+      <c r="H4">
         <v>130</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
         <v>9</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" t="s">
         <v>16</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
         <v>13</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
         <v>55</v>
       </c>
-      <c r="E5" t="s">
+      <c r="F5" t="s">
         <v>61</v>
       </c>
-      <c r="F5" t="s">
+      <c r="G5" t="s">
         <v>6</v>
       </c>
-      <c r="G5">
+      <c r="H5">
         <v>150</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
         <v>10</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C6" t="s">
         <v>17</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
         <v>14</v>
       </c>
-      <c r="D6" t="s">
+      <c r="E6" t="s">
         <v>20</v>
       </c>
-      <c r="E6" t="s">
+      <c r="F6" t="s">
         <v>21</v>
       </c>
-      <c r="F6" t="s">
+      <c r="G6" t="s">
         <v>6</v>
       </c>
-      <c r="G6">
+      <c r="H6">
         <v>200</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
         <v>18</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C7" t="s">
         <v>16</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" t="s">
         <v>13</v>
       </c>
-      <c r="D7" t="s">
+      <c r="E7" t="s">
         <v>55</v>
       </c>
-      <c r="E7" t="s">
+      <c r="F7" t="s">
         <v>61</v>
       </c>
-      <c r="F7" t="s">
+      <c r="G7" t="s">
         <v>6</v>
       </c>
-      <c r="G7">
+      <c r="H7">
         <v>170</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
         <v>19</v>
       </c>
-      <c r="B8" t="s">
+      <c r="C8" t="s">
         <v>17</v>
       </c>
-      <c r="C8" t="s">
+      <c r="D8" t="s">
         <v>14</v>
       </c>
-      <c r="D8" t="s">
+      <c r="E8" t="s">
         <v>20</v>
       </c>
-      <c r="E8" t="s">
+      <c r="F8" t="s">
         <v>22</v>
       </c>
-      <c r="F8" t="s">
+      <c r="G8" t="s">
         <v>6</v>
       </c>
-      <c r="G8">
+      <c r="H8">
         <v>210</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
         <v>23</v>
       </c>
-      <c r="B9" t="s">
+      <c r="C9" t="s">
         <v>16</v>
       </c>
-      <c r="C9" t="s">
+      <c r="D9" t="s">
         <v>13</v>
       </c>
-      <c r="D9" t="s">
+      <c r="E9" t="s">
         <v>55</v>
       </c>
-      <c r="E9" t="s">
+      <c r="F9" t="s">
         <v>61</v>
       </c>
-      <c r="F9" t="s">
+      <c r="G9" t="s">
         <v>6</v>
       </c>
-      <c r="G9">
+      <c r="H9">
         <v>310</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
         <v>25</v>
       </c>
-      <c r="B10" t="s">
+      <c r="C10" t="s">
         <v>40</v>
       </c>
-      <c r="C10" t="s">
+      <c r="D10" t="s">
         <v>41</v>
       </c>
-      <c r="D10" t="s">
+      <c r="E10" t="s">
         <v>48</v>
       </c>
-      <c r="E10" t="s">
+      <c r="F10" t="s">
         <v>49</v>
       </c>
-      <c r="F10" t="s">
+      <c r="G10" t="s">
         <v>47</v>
       </c>
-      <c r="G10">
+      <c r="H10">
         <v>768</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
         <v>24</v>
       </c>
-      <c r="B11" t="s">
+      <c r="C11" t="s">
         <v>39</v>
       </c>
-      <c r="C11" t="s">
+      <c r="D11" t="s">
         <v>43</v>
       </c>
-      <c r="D11" t="s">
+      <c r="E11" t="s">
         <v>50</v>
       </c>
-      <c r="E11" t="s">
+      <c r="F11" t="s">
         <v>51</v>
       </c>
-      <c r="F11" t="s">
+      <c r="G11" t="s">
         <v>74</v>
       </c>
-      <c r="G11">
+      <c r="H11">
         <v>400</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
         <v>26</v>
       </c>
-      <c r="B12" t="s">
+      <c r="C12" t="s">
         <v>40</v>
       </c>
-      <c r="C12" t="s">
+      <c r="D12" t="s">
         <v>42</v>
       </c>
-      <c r="D12" t="s">
+      <c r="E12" t="s">
         <v>52</v>
       </c>
-      <c r="E12" t="s">
+      <c r="F12" t="s">
         <v>53</v>
       </c>
-      <c r="F12" t="s">
+      <c r="G12" t="s">
         <v>47</v>
       </c>
-      <c r="G12">
+      <c r="H12">
         <v>648</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
         <v>27</v>
       </c>
-      <c r="B13" t="s">
+      <c r="C13" t="s">
         <v>36</v>
       </c>
-      <c r="C13" t="s">
+      <c r="D13" t="s">
         <v>41</v>
       </c>
-      <c r="D13" t="s">
+      <c r="E13" t="s">
         <v>55</v>
       </c>
-      <c r="E13" t="s">
+      <c r="F13" t="s">
         <v>54</v>
       </c>
-      <c r="F13" t="s">
+      <c r="G13" t="s">
         <v>70</v>
       </c>
-      <c r="G13">
+      <c r="H13">
         <v>120</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
         <v>27</v>
       </c>
-      <c r="B14" t="s">
+      <c r="C14" t="s">
         <v>36</v>
       </c>
-      <c r="C14" t="s">
+      <c r="D14" t="s">
         <v>41</v>
       </c>
-      <c r="D14" t="s">
+      <c r="E14" t="s">
         <v>55</v>
       </c>
-      <c r="E14" t="s">
+      <c r="F14" t="s">
         <v>56</v>
       </c>
-      <c r="F14" t="s">
+      <c r="G14" t="s">
         <v>70</v>
       </c>
-      <c r="G14">
+      <c r="H14">
         <v>150</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
         <v>28</v>
       </c>
-      <c r="B15" t="s">
+      <c r="C15" t="s">
         <v>39</v>
       </c>
-      <c r="C15" t="s">
+      <c r="D15" t="s">
         <v>46</v>
       </c>
-      <c r="D15" t="s">
+      <c r="E15" t="s">
         <v>57</v>
       </c>
-      <c r="E15" t="s">
+      <c r="F15" t="s">
         <v>58</v>
       </c>
-      <c r="F15" t="s">
+      <c r="G15" t="s">
         <v>73</v>
       </c>
-      <c r="G15">
+      <c r="H15">
         <v>190</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" t="s">
         <v>29</v>
       </c>
-      <c r="B16" t="s">
+      <c r="C16" t="s">
         <v>38</v>
       </c>
-      <c r="C16" t="s">
+      <c r="D16" t="s">
         <v>46</v>
       </c>
-      <c r="D16" t="s">
+      <c r="E16" t="s">
         <v>59</v>
       </c>
-      <c r="E16" t="s">
+      <c r="F16" t="s">
         <v>49</v>
       </c>
-      <c r="F16" t="s">
+      <c r="G16" t="s">
         <v>72</v>
       </c>
-      <c r="G16">
+      <c r="H16">
         <v>490</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" t="s">
         <v>30</v>
       </c>
-      <c r="B17" t="s">
+      <c r="C17" t="s">
         <v>37</v>
       </c>
-      <c r="C17" t="s">
+      <c r="D17" t="s">
         <v>44</v>
       </c>
-      <c r="D17" t="s">
+      <c r="E17" t="s">
         <v>60</v>
       </c>
-      <c r="E17" t="s">
+      <c r="F17" t="s">
         <v>61</v>
       </c>
-      <c r="F17" t="s">
+      <c r="G17" t="s">
         <v>71</v>
       </c>
-      <c r="G17">
+      <c r="H17">
         <v>220</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18" t="s">
         <v>31</v>
       </c>
-      <c r="B18" t="s">
+      <c r="C18" t="s">
         <v>36</v>
       </c>
-      <c r="C18" t="s">
+      <c r="D18" t="s">
         <v>44</v>
       </c>
-      <c r="D18" t="s">
+      <c r="E18" t="s">
         <v>63</v>
       </c>
-      <c r="E18" t="s">
+      <c r="F18" t="s">
         <v>62</v>
       </c>
-      <c r="F18" t="s">
+      <c r="G18" t="s">
         <v>70</v>
       </c>
-      <c r="G18">
+      <c r="H18">
         <v>90</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19" t="s">
         <v>32</v>
       </c>
-      <c r="B19" t="s">
+      <c r="C19" t="s">
         <v>35</v>
       </c>
-      <c r="C19" t="s">
+      <c r="D19" t="s">
         <v>45</v>
       </c>
-      <c r="D19" t="s">
+      <c r="E19" t="s">
         <v>64</v>
       </c>
-      <c r="E19" t="s">
+      <c r="F19" t="s">
         <v>65</v>
       </c>
-      <c r="F19" t="s">
+      <c r="G19" t="s">
         <v>69</v>
       </c>
-      <c r="G19">
+      <c r="H19">
         <v>210</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20" t="s">
         <v>33</v>
       </c>
-      <c r="B20" t="s">
+      <c r="C20" t="s">
         <v>34</v>
       </c>
-      <c r="C20" t="s">
+      <c r="D20" t="s">
         <v>45</v>
       </c>
-      <c r="D20" t="s">
+      <c r="E20" t="s">
         <v>66</v>
       </c>
-      <c r="E20" t="s">
+      <c r="F20" t="s">
         <v>67</v>
       </c>
-      <c r="F20" t="s">
+      <c r="G20" t="s">
         <v>68</v>
       </c>
-      <c r="G20">
+      <c r="H20">
         <v>200</v>
       </c>
     </row>

</xml_diff>